<commit_message>
added sheet for marking
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@1225 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/connectathons/atlantaMay2013/Connectathon marking.xlsx
+++ b/connectathons/atlantaMay2013/Connectathon marking.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="255" windowWidth="25365" windowHeight="16215" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="registration" sheetId="4" r:id="rId1"/>
     <sheet name="Individual" sheetId="2" r:id="rId2"/>
     <sheet name="summary by scenario" sheetId="1" r:id="rId3"/>
+    <sheet name="scorecard" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="73">
   <si>
     <t>Clients</t>
   </si>
@@ -195,13 +196,58 @@
   </si>
   <si>
     <t>Eliot Muir</t>
+  </si>
+  <si>
+    <t>participant 1</t>
+  </si>
+  <si>
+    <t>David Browser</t>
+  </si>
+  <si>
+    <t>David Android</t>
+  </si>
+  <si>
+    <t>Claude</t>
+  </si>
+  <si>
+    <t>Rolim</t>
+  </si>
+  <si>
+    <t>Healthfile</t>
+  </si>
+  <si>
+    <t>Eliot</t>
+  </si>
+  <si>
+    <t>Scenario1</t>
+  </si>
+  <si>
+    <t>Scenario2</t>
+  </si>
+  <si>
+    <t>Scenario3</t>
+  </si>
+  <si>
+    <t>Scenario4</t>
+  </si>
+  <si>
+    <t>Result scorecard</t>
+  </si>
+  <si>
+    <t>Place the representation (json / xml) in the cell</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Claim extensions in problem processing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -259,6 +305,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -283,7 +336,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -299,8 +352,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -316,8 +377,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -325,6 +387,10 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -332,6 +398,10 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -668,41 +738,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.375" customWidth="1"/>
-    <col min="2" max="2" width="4.375" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="5.875" customWidth="1"/>
-    <col min="7" max="7" width="6.125" customWidth="1"/>
-    <col min="8" max="9" width="6.875" customWidth="1"/>
-    <col min="10" max="10" width="6.125" customWidth="1"/>
-    <col min="11" max="11" width="33.375" customWidth="1"/>
-    <col min="12" max="13" width="5.625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" customWidth="1"/>
+    <col min="8" max="9" width="6.83203125" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" customWidth="1"/>
+    <col min="11" max="11" width="33.33203125" customWidth="1"/>
+    <col min="12" max="13" width="5.6640625" customWidth="1"/>
     <col min="14" max="14" width="6.5" customWidth="1"/>
     <col min="15" max="15" width="5" customWidth="1"/>
     <col min="16" max="16" width="5.5" customWidth="1"/>
     <col min="17" max="17" width="4" customWidth="1"/>
-    <col min="18" max="18" width="5.375" customWidth="1"/>
-    <col min="19" max="19" width="6.375" customWidth="1"/>
+    <col min="18" max="18" width="5.33203125" customWidth="1"/>
+    <col min="19" max="19" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21">
       <c r="B2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21">
       <c r="T5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21">
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
@@ -729,7 +799,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21">
       <c r="E8" t="s">
         <v>20</v>
       </c>
@@ -758,7 +828,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21">
       <c r="E9" t="s">
         <v>1</v>
       </c>
@@ -808,7 +878,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21">
       <c r="T10">
         <v>4</v>
       </c>
@@ -816,7 +886,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21">
       <c r="C12" t="s">
         <v>4</v>
       </c>
@@ -839,7 +909,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21">
       <c r="C13" t="s">
         <v>5</v>
       </c>
@@ -862,7 +932,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21">
       <c r="C14" t="s">
         <v>38</v>
       </c>
@@ -873,7 +943,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21">
       <c r="C15" t="s">
         <v>53</v>
       </c>
@@ -884,16 +954,16 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21">
       <c r="C16" t="s">
         <v>55</v>
       </c>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:19">
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:19">
       <c r="C18" t="s">
         <v>37</v>
       </c>
@@ -910,42 +980,42 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:19">
       <c r="C20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:19">
       <c r="C21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:19">
       <c r="C22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:19">
       <c r="C23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:19">
       <c r="C24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:19">
       <c r="C25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:19">
       <c r="C26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:19">
       <c r="C27" t="s">
         <v>46</v>
       </c>
@@ -962,7 +1032,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:19">
       <c r="C28" t="s">
         <v>56</v>
       </c>
@@ -985,32 +1055,32 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:19">
       <c r="C29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:19">
       <c r="C30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:19">
       <c r="C31" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:19">
       <c r="C32" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:19">
       <c r="C33" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:19">
       <c r="C34" t="s">
         <v>52</v>
       </c>
@@ -1024,7 +1094,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:19">
       <c r="C35" t="s">
         <v>57</v>
       </c>
@@ -1051,28 +1121,28 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="27.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="28" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="17.875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="3.875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="3.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
     <col min="7" max="7" width="16.5" customWidth="1"/>
     <col min="8" max="8" width="4" style="3" customWidth="1"/>
     <col min="9" max="10" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:13" ht="28" customHeight="1">
       <c r="B1" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="12"/>
       <c r="H1" s="12"/>
     </row>
-    <row r="2" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" ht="28" customHeight="1">
       <c r="E2" s="12"/>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="2:13" s="11" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:13" s="11" customFormat="1" ht="28" customHeight="1">
       <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
@@ -1080,11 +1150,11 @@
       <c r="E3" s="13"/>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" ht="28" customHeight="1">
       <c r="E4" s="12"/>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="2:13" s="7" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" s="7" customFormat="1" ht="28" customHeight="1">
       <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1099,7 +1169,7 @@
       </c>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="28" customHeight="1">
       <c r="E6" s="5"/>
       <c r="F6" t="s">
         <v>6</v>
@@ -1115,7 +1185,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="28" customHeight="1">
       <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
@@ -1129,7 +1199,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="28" customHeight="1">
       <c r="D8" t="s">
         <v>2</v>
       </c>
@@ -1140,7 +1210,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="28" customHeight="1">
       <c r="D9" t="s">
         <v>17</v>
       </c>
@@ -1151,7 +1221,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="2:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="9" customHeight="1">
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1159,7 +1229,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="28" customHeight="1">
       <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
@@ -1173,7 +1243,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="28" customHeight="1">
       <c r="D12" t="s">
         <v>2</v>
       </c>
@@ -1184,7 +1254,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" ht="28" customHeight="1">
       <c r="D13" t="s">
         <v>17</v>
       </c>
@@ -1195,7 +1265,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" ht="12" customHeight="1">
       <c r="E14" s="5"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -1203,7 +1273,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" ht="28" customHeight="1">
       <c r="C15" s="9" t="s">
         <v>13</v>
       </c>
@@ -1217,7 +1287,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" ht="28" customHeight="1">
       <c r="D16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1228,14 +1298,14 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="3:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:8" ht="28" customHeight="1">
       <c r="D17" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="19" spans="3:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:8" ht="28" customHeight="1">
       <c r="C19" s="9" t="s">
         <v>34</v>
       </c>
@@ -1243,12 +1313,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" ht="28" customHeight="1">
       <c r="D20" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="3:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" ht="28" customHeight="1">
       <c r="D21" t="s">
         <v>17</v>
       </c>
@@ -1269,44 +1339,44 @@
   <dimension ref="B1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="27.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="28" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="17.875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="3.875" style="3" customWidth="1"/>
-    <col min="6" max="7" width="10.125" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="3.83203125" style="3" customWidth="1"/>
+    <col min="6" max="7" width="10.1640625" customWidth="1"/>
     <col min="8" max="8" width="4" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.875" customWidth="1"/>
-    <col min="10" max="10" width="9.375" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" ht="28" customHeight="1">
       <c r="B1" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="12"/>
       <c r="H1" s="12"/>
     </row>
-    <row r="2" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" ht="28" customHeight="1">
       <c r="E2" s="12"/>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" ht="28" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="12"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" ht="28" customHeight="1">
       <c r="E4" s="12"/>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="2:13" s="7" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" s="7" customFormat="1" ht="28" customHeight="1">
       <c r="C5" s="7" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>3</v>
@@ -1319,7 +1389,7 @@
       </c>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="28" customHeight="1">
       <c r="E6" s="5"/>
       <c r="F6" t="s">
         <v>6</v>
@@ -1335,7 +1405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="28" customHeight="1">
       <c r="C7" s="9" t="s">
         <v>37</v>
       </c>
@@ -1349,7 +1419,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="28" customHeight="1">
       <c r="D8" t="s">
         <v>2</v>
       </c>
@@ -1360,7 +1430,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="28" customHeight="1">
       <c r="E9" s="5"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1368,7 +1438,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="28" customHeight="1">
       <c r="C10" s="9" t="s">
         <v>28</v>
       </c>
@@ -1382,7 +1452,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="28" customHeight="1">
       <c r="D11" t="s">
         <v>2</v>
       </c>
@@ -1393,7 +1463,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="28" customHeight="1">
       <c r="E12" s="5"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -1401,7 +1471,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" ht="28" customHeight="1">
       <c r="C13" s="9" t="s">
         <v>29</v>
       </c>
@@ -1415,7 +1485,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" ht="28" customHeight="1">
       <c r="D14" s="1" t="s">
         <v>2</v>
       </c>
@@ -1426,9 +1496,244 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" ht="28" customHeight="1">
       <c r="E15" s="5"/>
       <c r="H15" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:U26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="7.5" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" customWidth="1"/>
+    <col min="10" max="11" width="6.83203125" customWidth="1"/>
+    <col min="12" max="12" width="5.83203125" customWidth="1"/>
+    <col min="13" max="13" width="9.83203125" customWidth="1"/>
+    <col min="14" max="14" width="7.83203125" customWidth="1"/>
+    <col min="15" max="15" width="5.6640625" customWidth="1"/>
+    <col min="16" max="16" width="6.83203125" customWidth="1"/>
+    <col min="17" max="17" width="9.83203125" customWidth="1"/>
+    <col min="19" max="19" width="6.5" customWidth="1"/>
+    <col min="20" max="20" width="7.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:21" ht="23">
+      <c r="A2" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="2" customFormat="1">
+      <c r="E4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S5" t="s">
+        <v>53</v>
+      </c>
+      <c r="T5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="B8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T8" t="s">
+        <v>2</v>
+      </c>
+      <c r="U8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" t="s">
+        <v>2</v>
+      </c>
+      <c r="T9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="B11" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="B12" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="B13" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>